<commit_message>
Cleaning up extra comments
</commit_message>
<xml_diff>
--- a/sample_data/sales/pending/John Doe 101.xlsx
+++ b/sample_data/sales/pending/John Doe 101.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65bed8121c905128/Desktop/Tiktok/Tutorial/update_tutorial/office_automations/sample_data/sales/pending/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65bed8121c905128/Desktop/Tiktok/Sample Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC1048AD119B5F785BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AD264C6-0DAA-415E-9A2F-71A82F65C184}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_F25DC773A252ABDACC1048AD119B5F785BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B81CB30-B650-4B34-B706-8D4746D443A1}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="4635" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="1320" windowWidth="33705" windowHeight="18480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
@@ -86,9 +86,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -113,13 +114,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{87017C6C-82B5-46D4-98CA-952582F68961}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="6">
+  <queryTableRefresh nextId="5">
     <queryTableFields count="4">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
       <queryTableField id="2" name="Employee Name" tableColumnId="2"/>
@@ -409,7 +406,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,9 +433,9 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45355</v>
-      </c>
-      <c r="B2" t="s">
+        <v>45359</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2">
@@ -450,9 +447,9 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45356</v>
-      </c>
-      <c r="B3" t="s">
+        <v>45360</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3">
@@ -464,9 +461,9 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45357</v>
-      </c>
-      <c r="B4" t="s">
+        <v>45361</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -478,9 +475,9 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45358</v>
-      </c>
-      <c r="B5" t="s">
+        <v>45362</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5">
@@ -492,9 +489,9 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45359</v>
-      </c>
-      <c r="B6" t="s">
+        <v>45363</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6">

</xml_diff>